<commit_message>
added new bar conference page
</commit_message>
<xml_diff>
--- a/test/cbb_2020.xlsx
+++ b/test/cbb_2020.xlsx
@@ -9,23 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="cbb_2020" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">cbb_2020!$S$2:$S$76</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">cbb_2020!$W$2:$W$76</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">cbb_2020!$S$2:$S$76</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">cbb_2020!$W$2:$W$76</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="106">
   <si>
     <t>RK</t>
   </si>
@@ -340,6 +334,9 @@
   </si>
   <si>
     <t>AVRB</t>
+  </si>
+  <si>
+    <t>BOTH</t>
   </si>
 </sst>
 </file>
@@ -1878,8 +1875,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.25821697480764172"/>
-                  <c:y val="-0.33306469680980599"/>
+                  <c:x val="0.26446187566144941"/>
+                  <c:y val="-0.11416251319100573"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2148,234 +2145,234 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>cbb_2020!$N$2:$N$76</c:f>
+              <c:f>cbb_2020!$M$2:$M$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="75"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>34.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>30.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="18">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>34.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>32.200000000000003</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="37">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>23.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25.7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>29.1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>33.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>32.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>31.3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>30.7</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>32.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>27.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>25.1</c:v>
+                </c:pt>
+                <c:pt idx="61">
                   <c:v>30.9</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>28.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>31.9</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>25.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>34.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30.7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>25.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>25.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>27.6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>25.9</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>27.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>26.6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>27.9</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>25.7</c:v>
-                </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="62">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>35.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>35.1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>32.1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>31.6</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>31.4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>26.4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>31.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>25.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>29.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>24.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>29.3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>26.4</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>29.8</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>27.6</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>29.2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>27.4</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>32.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>29.6</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>31.6</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>30.2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>30.2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>24.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>30.4</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>25.4</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>28.4</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>27.6</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>31.4</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>28.7</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>30.2</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>25.9</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>31.1</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>23.9</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>27.8</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>31.8</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>27.9</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>28.6</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>25.4</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>26.9</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>26.3</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>28.5</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>27.4</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>27.4</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>28.5</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>28.3</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>31.4</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>28.6</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>30.1</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>30.1</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>27.7</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>27.8</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>31.8</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>29.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2481,7 +2478,7 @@
         <c:axId val="1547016079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="35"/>
+          <c:max val="40"/>
           <c:min val="20"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6613,16 +6610,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>75078</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>97490</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>175932</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>175931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>17928</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>145115</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>421341</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>33056</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6643,16 +6640,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>313765</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>256615</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>114860</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>99733</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>137272</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6707,16 +6704,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>481852</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>100853</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>67234</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>424702</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>148478</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>10084</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>159684</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7003,10 +7000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y76"/>
+  <dimension ref="A1:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AC2:AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7014,7 +7011,7 @@
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7087,8 +7084,29 @@
       <c r="X1" t="s">
         <v>104</v>
       </c>
+      <c r="AB1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -7167,8 +7185,35 @@
         <f>F2-G2</f>
         <v>23.399999999999991</v>
       </c>
+      <c r="AB2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="1">
+        <f>AVERAGE(F2:F16)</f>
+        <v>107.64666666666668</v>
+      </c>
+      <c r="AD2" s="1">
+        <f>AVERAGE(G2:G16)</f>
+        <v>95.899999999999991</v>
+      </c>
+      <c r="AE2" s="1">
+        <f>AVERAGE(M2:M16)</f>
+        <v>28.90666666666667</v>
+      </c>
+      <c r="AF2" s="1">
+        <f>AVERAGE(Q2:Q16)</f>
+        <v>49.533333333333331</v>
+      </c>
+      <c r="AG2" s="1">
+        <f>AVERAGE(S2:S16)</f>
+        <v>32.846666666666671</v>
+      </c>
+      <c r="AH2" s="1">
+        <f>AC2-AD2</f>
+        <v>11.746666666666684</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -7247,8 +7292,35 @@
         <f t="shared" ref="Y3:Y66" si="2">F3-G3</f>
         <v>21.199999999999989</v>
       </c>
+      <c r="AB3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="1">
+        <f>AVERAGE(F17:F30)</f>
+        <v>110.66428571428571</v>
+      </c>
+      <c r="AD3" s="1">
+        <f>AVERAGE(G17:G30)</f>
+        <v>94.285714285714292</v>
+      </c>
+      <c r="AE3" s="1">
+        <f>AVERAGE(M17:M30)</f>
+        <v>29.728571428571431</v>
+      </c>
+      <c r="AF3" s="1">
+        <f>AVERAGE(Q17:Q30)</f>
+        <v>49.578571428571429</v>
+      </c>
+      <c r="AG3" s="1">
+        <f>AVERAGE(S17:S30)</f>
+        <v>33.064285714285717</v>
+      </c>
+      <c r="AH3" s="1">
+        <f t="shared" ref="AH3:AH7" si="3">AC3-AD3</f>
+        <v>16.378571428571419</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -7327,8 +7399,35 @@
         <f t="shared" si="2"/>
         <v>18.700000000000003</v>
       </c>
+      <c r="AB4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>AVERAGE(F31:F40)</f>
+        <v>108.32000000000001</v>
+      </c>
+      <c r="AD4" s="1">
+        <f>AVERAGE(G31:G40)</f>
+        <v>92.940000000000012</v>
+      </c>
+      <c r="AE4" s="1">
+        <f>AVERAGE(M31:M40)</f>
+        <v>30.7</v>
+      </c>
+      <c r="AF4" s="1">
+        <f>AVERAGE(Q31:Q40)</f>
+        <v>49.339999999999996</v>
+      </c>
+      <c r="AG4" s="1">
+        <f>AVERAGE(S31:S40)</f>
+        <v>32.850000000000009</v>
+      </c>
+      <c r="AH4" s="1">
+        <f t="shared" si="3"/>
+        <v>15.379999999999995</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>34</v>
       </c>
@@ -7407,8 +7506,35 @@
         <f t="shared" si="2"/>
         <v>14.400000000000006</v>
       </c>
+      <c r="AB5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC5" s="1">
+        <f>AVERAGE(F41:F50)</f>
+        <v>110.86999999999998</v>
+      </c>
+      <c r="AD5" s="1">
+        <f>AVERAGE(G41:G50)</f>
+        <v>94.960000000000008</v>
+      </c>
+      <c r="AE5" s="1">
+        <f>AVERAGE(M41:M50)</f>
+        <v>29.78</v>
+      </c>
+      <c r="AF5" s="1">
+        <f>AVERAGE(Q41:Q50)</f>
+        <v>49.379999999999995</v>
+      </c>
+      <c r="AG5" s="1">
+        <f>AVERAGE(S41:S50)</f>
+        <v>34.260000000000005</v>
+      </c>
+      <c r="AH5" s="1">
+        <f t="shared" si="3"/>
+        <v>15.909999999999968</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>44</v>
       </c>
@@ -7487,8 +7613,35 @@
         <f t="shared" si="2"/>
         <v>14.900000000000006</v>
       </c>
+      <c r="AB6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC6" s="1">
+        <f>AVERAGE(F51:F62)</f>
+        <v>107.23333333333335</v>
+      </c>
+      <c r="AD6" s="1">
+        <f>AVERAGE(G51:G62)</f>
+        <v>95.850000000000009</v>
+      </c>
+      <c r="AE6" s="1">
+        <f>AVERAGE(M51:M62)</f>
+        <v>28.600000000000005</v>
+      </c>
+      <c r="AF6" s="1">
+        <f>AVERAGE(Q51:Q62)</f>
+        <v>49.608333333333327</v>
+      </c>
+      <c r="AG6" s="1">
+        <f>AVERAGE(S51:S62)</f>
+        <v>34.124999999999993</v>
+      </c>
+      <c r="AH6" s="1">
+        <f t="shared" si="3"/>
+        <v>11.38333333333334</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>46</v>
       </c>
@@ -7567,8 +7720,35 @@
         <f t="shared" si="2"/>
         <v>14.099999999999994</v>
       </c>
+      <c r="AB7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7" s="1">
+        <f>AVERAGE(F63:F76)</f>
+        <v>108.74285714285713</v>
+      </c>
+      <c r="AD7" s="1">
+        <f>AVERAGE(G63:G76)</f>
+        <v>97.721428571428604</v>
+      </c>
+      <c r="AE7" s="1">
+        <f>AVERAGE(M63:M76)</f>
+        <v>30.664285714285711</v>
+      </c>
+      <c r="AF7" s="1">
+        <f>AVERAGE(Q63:Q76)</f>
+        <v>51.135714285714286</v>
+      </c>
+      <c r="AG7" s="1">
+        <f>AVERAGE(S63:S76)</f>
+        <v>32.207142857142863</v>
+      </c>
+      <c r="AH7" s="1">
+        <f t="shared" si="3"/>
+        <v>11.02142857142853</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>51</v>
       </c>
@@ -7648,7 +7828,7 @@
         <v>12.299999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>55</v>
       </c>
@@ -7728,7 +7908,7 @@
         <v>12.700000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>71</v>
       </c>
@@ -7808,7 +7988,7 @@
         <v>10.299999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>78</v>
       </c>
@@ -7888,7 +8068,7 @@
         <v>9.9000000000000057</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>101</v>
       </c>
@@ -7968,7 +8148,7 @@
         <v>7.2000000000000028</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>102</v>
       </c>
@@ -8048,7 +8228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>118</v>
       </c>
@@ -8128,7 +8308,7 @@
         <v>5.2000000000000028</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>123</v>
       </c>
@@ -8208,7 +8388,7 @@
         <v>4.4000000000000057</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>167</v>
       </c>
@@ -12356,15 +12536,15 @@
         <v>-0.5</v>
       </c>
       <c r="W67" s="1">
-        <f t="shared" ref="W67:W76" si="3">E67/D67 * 100</f>
+        <f t="shared" ref="W67:W76" si="4">E67/D67 * 100</f>
         <v>64.516129032258064</v>
       </c>
       <c r="X67">
-        <f t="shared" ref="X67:X76" si="4">AVERAGE(M67,N67)</f>
+        <f t="shared" ref="X67:X76" si="5">AVERAGE(M67,N67)</f>
         <v>32.65</v>
       </c>
       <c r="Y67">
-        <f t="shared" ref="Y67:Y76" si="5">F67-G67</f>
+        <f t="shared" ref="Y67:Y76" si="6">F67-G67</f>
         <v>13.799999999999997</v>
       </c>
     </row>
@@ -12436,15 +12616,15 @@
         <v>-1.3</v>
       </c>
       <c r="W68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
       <c r="X68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26.45</v>
       </c>
       <c r="Y68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.800000000000011</v>
       </c>
     </row>
@@ -12516,15 +12696,15 @@
         <v>-3.8</v>
       </c>
       <c r="W69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51.612903225806448</v>
       </c>
       <c r="X69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.35</v>
       </c>
       <c r="Y69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.200000000000003</v>
       </c>
     </row>
@@ -12596,15 +12776,15 @@
         <v>-2.4</v>
       </c>
       <c r="W70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58.064516129032263</v>
       </c>
       <c r="X70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.35</v>
       </c>
       <c r="Y70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.5</v>
       </c>
     </row>
@@ -12676,15 +12856,15 @@
         <v>-2.1</v>
       </c>
       <c r="W71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54.838709677419352</v>
       </c>
       <c r="X71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.3</v>
       </c>
       <c r="Y71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.799999999999997</v>
       </c>
     </row>
@@ -12756,15 +12936,15 @@
         <v>-4.2</v>
       </c>
       <c r="W72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51.612903225806448</v>
       </c>
       <c r="X72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.85</v>
       </c>
       <c r="Y72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.6000000000000085</v>
       </c>
     </row>
@@ -12836,15 +13016,15 @@
         <v>-4.5999999999999996</v>
       </c>
       <c r="W73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48.387096774193552</v>
       </c>
       <c r="X73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.549999999999997</v>
       </c>
       <c r="Y73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.0999999999999943</v>
       </c>
     </row>
@@ -12916,15 +13096,15 @@
         <v>-5.5</v>
       </c>
       <c r="W74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46.875</v>
       </c>
       <c r="X74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.1</v>
       </c>
       <c r="Y74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
     </row>
@@ -12996,15 +13176,15 @@
         <v>-3.9</v>
       </c>
       <c r="W75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53.333333333333336</v>
       </c>
       <c r="X75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31.55</v>
       </c>
       <c r="Y75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7999999999999972</v>
       </c>
     </row>
@@ -13076,15 +13256,15 @@
         <v>-10</v>
       </c>
       <c r="W76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34.375</v>
       </c>
       <c r="X76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.4</v>
       </c>
       <c r="Y76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1999999999999886</v>
       </c>
     </row>

</xml_diff>